<commit_message>
capitulo 4 código java
</commit_message>
<xml_diff>
--- a/datosDist.xlsx
+++ b/datosDist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MRS\Documents\Belen\ucm\5\TFG infor\TFG-1920-DiscapacidadVisual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MRS\Documents\Belen\ucm\5\TFG infor\git\TFG-1920-DiscapacidadVisual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45A9283-61D3-4524-9ECD-76A204066725}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58049402-019A-4BC9-A601-60A4FAF3B6E5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{BACB8FA7-8DF2-4461-B1D7-FE215F08741E}"/>
   </bookViews>
@@ -36,9 +36,6 @@
     <t>beacon: CPne a 2m</t>
   </si>
   <si>
-    <t>beacon: eAaw a 0,5 m</t>
-  </si>
-  <si>
     <t>beacon: 8v2c a 4m</t>
   </si>
   <si>
@@ -63,25 +60,28 @@
     <t>eAaw (pegado al movil, a milimetros)</t>
   </si>
   <si>
-    <t>8v2c (a 64 cm, uno encima del otro )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">beacon: eAaw a 0,5 </t>
-  </si>
-  <si>
-    <t>beacon: eAaw a 5cm aprox</t>
-  </si>
-  <si>
-    <t>beacon: eAaw pegado al movil, a milimetros</t>
-  </si>
-  <si>
-    <t>beacon: CPne a 2 metros largos</t>
-  </si>
-  <si>
     <t>beacon: CPne a 5m</t>
   </si>
   <si>
-    <t>beacon: CPne a 64 cm,uno encima del otro</t>
+    <t>beacon: CPne a 2,5m</t>
+  </si>
+  <si>
+    <t>beacon: CPne a 64cm</t>
+  </si>
+  <si>
+    <t>beacon: eAaw a 5cm</t>
+  </si>
+  <si>
+    <t>beacon: eAaw a 0,5m</t>
+  </si>
+  <si>
+    <t>beacon: eAaw a 7mm</t>
+  </si>
+  <si>
+    <t>beacon: 8v2c a 64cm</t>
+  </si>
+  <si>
+    <t>beacon: Cpne a 64cm</t>
   </si>
 </sst>
 </file>
@@ -191,7 +191,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja2!$B$4</c:f>
+              <c:f>Hoja2!$C$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -316,7 +316,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja2!$B$5:$B$35</c:f>
+              <c:f>Hoja2!$C$5:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
@@ -2049,7 +2049,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>8v2c (a 64 cm, uno encima del otro )</c:v>
+                  <c:v>beacon: 8v2c a 64cm</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2777,7 +2777,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>8v2c (a 64 cm, uno encima del otro )</c:v>
+                  <c:v>beacon: 8v2c a 64cm</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3254,7 +3254,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>beacon: CPne(a 64 cm,uno encima del otro)</c:v>
+                  <c:v>beacon: Cpne a 64cm</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3959,1239 +3959,6 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="es-ES"/>
-              <a:t>beacon</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="es-ES" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="es-ES"/>
-              <a:t>CPne</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hoja2!$B$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>beacon: CPne a 2m</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Hoja2!$A$5:$A$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>115</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>125</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>135</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>155</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja2!$B$5:$B$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
-                <c:pt idx="0">
-                  <c:v>2.22080465534951</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.3190883356183201</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.7155711877451401</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.0388873079462901</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.3190883356183201</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.5724175935226301</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.2074340059003399</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.1048704445411901</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.1048704445411901</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.7155711877451401</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.3190883356183201</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.87746271403461995</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.67206293706674802</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2.22080465534951</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.4174822379066199</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.87077681793044</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.87077681793044</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2.0388873079462901</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.1048704445411901</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.2074340059003399</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.87746271403461995</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.1048704445411901</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2.4174822379066199</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2.0388873079462901</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.87077681793044</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1.87077681793044</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2.22080465534951</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1.0107600000000001</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.87746271403461995</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1.0107600000000001</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1.5724175935226301</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D078-46A2-9A77-96503828AD9C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hoja2!$C$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>beacon: CPne a 2 metros largos</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Hoja2!$A$5:$A$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>115</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>125</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>135</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>155</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja2!$C$5:$C$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
-                <c:pt idx="0">
-                  <c:v>1.44051024859512</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.8592022614041501</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.5724175935226301</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.5724175935226301</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.1048704445411901</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.1048704445411901</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.5724175935226301</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.2074340059003399</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.0107600000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.44051024859512</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.33387481135659403</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.87746271403461995</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.38554328942953098</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2.8592022614041501</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.87746271403461995</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.38554328942953098</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2.6299270915773598</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.76860885253802902</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.33387481135659403</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2.4174822379066199</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.38554328942953098</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.38554328942953098</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2.0388873079462901</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.38554328942953098</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2.22080465534951</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.87746271403461995</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.38554328942953098</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1.87077681793044</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.87746271403461995</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.38554328942953098</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1.5724175935226301</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D078-46A2-9A77-96503828AD9C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hoja2!$D$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>beacon: CPne a 5m</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Hoja2!$A$5:$A$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>115</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>125</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>135</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>155</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja2!$D$5:$D$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
-                <c:pt idx="0">
-                  <c:v>1.7155711877451401</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.2074340059003399</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.8592022614041501</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.7155711877451401</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.8864239163560299</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.8864239163560299</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.44051024859512</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.3727904024403998</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.5724175935226301</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.5724175935226301</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.9679652700759802</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.7155711877451401</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4.6555048514850803</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4.6555048514850803</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.0388873079462901</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.6299270915773598</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2.6299270915773598</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3.1064292267626299</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3.65953171702269</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.2074340059003399</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3.9679652700759802</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3.1064292267626299</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.7155711877451401</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2.4174822379066199</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2.4174822379066199</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2.8592022614041501</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3.1064292267626299</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1.5724175935226301</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>3.9679652700759802</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1.7155711877451401</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1.87077681793044</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-D078-46A2-9A77-96503828AD9C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hoja2!$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>beacon: CPne a 64 cm,uno encima del otro</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Hoja2!$A$5:$A$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>115</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>125</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>135</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>155</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja2!$E$5:$E$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
-                <c:pt idx="0">
-                  <c:v>0.24879449996108899</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.214058315601307</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.44429992043324701</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.214058315601307</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.214058315601307</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.24879449996108899</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.18374956291599701</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.33387481135659403</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.33387481135659403</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.24879449996108899</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.33387481135659403</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.24879449996108899</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.28852395406988801</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.33387481135659403</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.38554328942953098</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.214058315601307</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.28852395406988801</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.33387481135659403</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.214058315601307</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.24879449996108899</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.28852395406988801</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.24879449996108899</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.33387481135659403</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.24879449996108899</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.28852395406988801</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.38554328942953098</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.24879449996108899</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.33387481135659403</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.38554328942953098</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.24879449996108899</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.33387481135659403</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-D078-46A2-9A77-96503828AD9C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="475163408"/>
-        <c:axId val="475159800"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="475163408"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="475159800"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="475159800"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="475163408"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="es-ES"/>
               <a:t>beacon eAaw</a:t>
             </a:r>
           </a:p>
@@ -5241,7 +4008,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>beacon: eAaw a 0,5 m</c:v>
+                  <c:v>beacon: eAaw a 0,5m</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5472,7 +4239,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>beacon: eAaw a 0,5 </c:v>
+                  <c:v>beacon: eAaw a 0,5m</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5703,7 +4470,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>beacon: eAaw a 5cm aprox</c:v>
+                  <c:v>beacon: eAaw a 5cm</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5934,7 +4701,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>beacon: eAaw pegado al movil, a milimetros</c:v>
+                  <c:v>beacon: eAaw a 7mm</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6358,7 +5125,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -7140,7 +5907,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>8v2c (a 64 cm, uno encima del otro )</c:v>
+                  <c:v>beacon: 8v2c a 64cm</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7564,6 +6331,1233 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>beacon CPne</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>beacon: CPne a 64cm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja2!$A$5:$A$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>155</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$B$5:$B$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>0.24879449996108899</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.214058315601307</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.44429992043324701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.214058315601307</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.214058315601307</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.24879449996108899</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.18374956291599701</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.33387481135659403</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.33387481135659403</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.24879449996108899</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.33387481135659403</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.24879449996108899</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.28852395406988801</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.33387481135659403</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.38554328942953098</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.214058315601307</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.28852395406988801</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.33387481135659403</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.214058315601307</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.24879449996108899</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.28852395406988801</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.24879449996108899</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.33387481135659403</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.24879449996108899</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.28852395406988801</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.38554328942953098</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.24879449996108899</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.33387481135659403</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.38554328942953098</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.24879449996108899</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.33387481135659403</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-25C7-43A8-A126-393D77E2163B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>beacon: CPne a 2m</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja2!$A$5:$A$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>155</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$C$5:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>2.22080465534951</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3190883356183201</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7155711877451401</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0388873079462901</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3190883356183201</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5724175935226301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2074340059003399</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1048704445411901</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1048704445411901</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.7155711877451401</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.3190883356183201</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.87746271403461995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.67206293706674802</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.22080465534951</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.4174822379066199</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.87077681793044</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.87077681793044</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.0388873079462901</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.1048704445411901</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.2074340059003399</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.87746271403461995</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.1048704445411901</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.4174822379066199</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.0388873079462901</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.87077681793044</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.87077681793044</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.22080465534951</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.0107600000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.87746271403461995</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.0107600000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.5724175935226301</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-25C7-43A8-A126-393D77E2163B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>beacon: CPne a 2,5m</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja2!$A$5:$A$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>155</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$D$5:$D$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>1.44051024859512</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8592022614041501</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5724175935226301</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5724175935226301</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1048704445411901</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1048704445411901</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5724175935226301</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2074340059003399</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0107600000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.44051024859512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.33387481135659403</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.87746271403461995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.38554328942953098</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.8592022614041501</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.87746271403461995</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.38554328942953098</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.6299270915773598</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.76860885253802902</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.33387481135659403</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.4174822379066199</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.38554328942953098</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.38554328942953098</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.0388873079462901</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.38554328942953098</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.22080465534951</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.87746271403461995</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.38554328942953098</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.87077681793044</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.87746271403461995</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.38554328942953098</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.5724175935226301</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-25C7-43A8-A126-393D77E2163B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>beacon: CPne a 5m</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja2!$A$5:$A$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>155</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$E$5:$E$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>1.7155711877451401</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2074340059003399</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8592022614041501</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7155711877451401</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.8864239163560299</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.8864239163560299</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.44051024859512</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.3727904024403998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5724175935226301</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5724175935226301</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.9679652700759802</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.7155711877451401</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.6555048514850803</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.6555048514850803</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.0388873079462901</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.6299270915773598</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.6299270915773598</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.1064292267626299</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.65953171702269</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.2074340059003399</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.9679652700759802</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.1064292267626299</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.7155711877451401</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.4174822379066199</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.4174822379066199</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.8592022614041501</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.1064292267626299</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.5724175935226301</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.9679652700759802</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.7155711877451401</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.87077681793044</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-25C7-43A8-A126-393D77E2163B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="422960904"/>
+        <c:axId val="422956968"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="422960904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="422956968"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="422956968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="422960904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -7623,7 +7617,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>beacon: eAaw a 0,5 m</c:v>
+                  <c:v>beacon: eAaw a 0,5m</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -21286,42 +21280,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>31749</xdr:colOff>
-      <xdr:row>98</xdr:row>
-      <xdr:rowOff>1588</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>793750</xdr:colOff>
-      <xdr:row>120</xdr:row>
-      <xdr:rowOff>7938</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="18" name="Gráfico 17">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFA0E7C9-0288-4037-A8CA-19BD793CC962}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>761999</xdr:colOff>
       <xdr:row>98</xdr:row>
@@ -21350,7 +21308,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -21375,6 +21333,42 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33953122-72E2-427B-A92E-A407DD150584}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>48946</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>8200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>683947</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>183885</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="15" name="Gráfico 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CD93C1B-CC0D-4FD3-BE3F-DB4E0CFFC6C8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -21694,8 +21688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD343F2-CB91-4D67-8970-030A01858BA8}">
   <dimension ref="A4:AX75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O65" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="V106" sqref="V106"/>
+    <sheetView tabSelected="1" topLeftCell="U83" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="Y99" sqref="Y99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21729,70 +21723,70 @@
   <sheetData>
     <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="I4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="J4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="K4" t="s">
         <v>12</v>
       </c>
       <c r="L4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y4" t="s">
         <v>2</v>
       </c>
-      <c r="Q4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R4" t="s">
-        <v>2</v>
-      </c>
-      <c r="S4" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y4" t="s">
+      <c r="AB4" t="s">
         <v>3</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AE4" t="s">
         <v>4</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AH4" t="s">
         <v>5</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AK4" t="s">
         <v>6</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AN4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AQ4" t="s">
         <v>7</v>
       </c>
-      <c r="AN4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AQ4" t="s">
+      <c r="AT4" t="s">
         <v>8</v>
       </c>
-      <c r="AT4" t="s">
-        <v>9</v>
-      </c>
       <c r="AW4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="AX4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.25">
@@ -21800,16 +21794,16 @@
         <v>5</v>
       </c>
       <c r="B5">
+        <v>0.24879449996108899</v>
+      </c>
+      <c r="C5">
         <v>2.22080465534951</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>1.44051024859512</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>1.7155711877451401</v>
-      </c>
-      <c r="E5">
-        <v>0.24879449996108899</v>
       </c>
       <c r="H5">
         <v>5</v>
@@ -21904,16 +21898,16 @@
         <v>10</v>
       </c>
       <c r="B6">
+        <v>0.214058315601307</v>
+      </c>
+      <c r="C6">
         <v>1.3190883356183201</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>2.8592022614041501</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>1.2074340059003399</v>
-      </c>
-      <c r="E6">
-        <v>0.214058315601307</v>
       </c>
       <c r="H6">
         <v>10</v>
@@ -22008,16 +22002,16 @@
         <v>15</v>
       </c>
       <c r="B7">
+        <v>0.44429992043324701</v>
+      </c>
+      <c r="C7">
         <v>1.7155711877451401</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>1.5724175935226301</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>2.8592022614041501</v>
-      </c>
-      <c r="E7">
-        <v>0.44429992043324701</v>
       </c>
       <c r="H7">
         <v>15</v>
@@ -22112,16 +22106,16 @@
         <v>20</v>
       </c>
       <c r="B8">
+        <v>0.214058315601307</v>
+      </c>
+      <c r="C8">
         <v>2.0388873079462901</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>1.5724175935226301</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>1.7155711877451401</v>
-      </c>
-      <c r="E8">
-        <v>0.214058315601307</v>
       </c>
       <c r="H8">
         <v>20</v>
@@ -22216,16 +22210,16 @@
         <v>25</v>
       </c>
       <c r="B9">
+        <v>0.214058315601307</v>
+      </c>
+      <c r="C9">
         <v>1.3190883356183201</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>1.1048704445411901</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>5.8864239163560299</v>
-      </c>
-      <c r="E9">
-        <v>0.214058315601307</v>
       </c>
       <c r="H9">
         <v>25</v>
@@ -22320,16 +22314,16 @@
         <v>30</v>
       </c>
       <c r="B10">
+        <v>0.24879449996108899</v>
+      </c>
+      <c r="C10">
         <v>1.5724175935226301</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>1.1048704445411901</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>5.8864239163560299</v>
-      </c>
-      <c r="E10">
-        <v>0.24879449996108899</v>
       </c>
       <c r="H10">
         <v>30</v>
@@ -22424,16 +22418,16 @@
         <v>35</v>
       </c>
       <c r="B11">
+        <v>0.18374956291599701</v>
+      </c>
+      <c r="C11">
         <v>1.2074340059003399</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>1.5724175935226301</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>1.44051024859512</v>
-      </c>
-      <c r="E11">
-        <v>0.18374956291599701</v>
       </c>
       <c r="H11">
         <v>35</v>
@@ -22528,16 +22522,16 @@
         <v>40</v>
       </c>
       <c r="B12">
+        <v>0.33387481135659403</v>
+      </c>
+      <c r="C12">
         <v>1.1048704445411901</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>1.2074340059003399</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>3.3727904024403998</v>
-      </c>
-      <c r="E12">
-        <v>0.33387481135659403</v>
       </c>
       <c r="H12">
         <v>40</v>
@@ -22632,16 +22626,16 @@
         <v>45</v>
       </c>
       <c r="B13">
+        <v>0.33387481135659403</v>
+      </c>
+      <c r="C13">
         <v>1.1048704445411901</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>1.0107600000000001</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>1.5724175935226301</v>
-      </c>
-      <c r="E13">
-        <v>0.33387481135659403</v>
       </c>
       <c r="H13">
         <v>45</v>
@@ -22736,16 +22730,16 @@
         <v>50</v>
       </c>
       <c r="B14">
+        <v>0.24879449996108899</v>
+      </c>
+      <c r="C14">
         <v>1.7155711877451401</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>1.44051024859512</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>1.5724175935226301</v>
-      </c>
-      <c r="E14">
-        <v>0.24879449996108899</v>
       </c>
       <c r="H14">
         <v>50</v>
@@ -22840,16 +22834,16 @@
         <v>55</v>
       </c>
       <c r="B15">
+        <v>0.33387481135659403</v>
+      </c>
+      <c r="C15">
         <v>1.3190883356183201</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>0.33387481135659403</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>3.9679652700759802</v>
-      </c>
-      <c r="E15">
-        <v>0.33387481135659403</v>
       </c>
       <c r="H15">
         <v>55</v>
@@ -22944,16 +22938,16 @@
         <v>60</v>
       </c>
       <c r="B16">
-        <v>0.87746271403461995</v>
+        <v>0.24879449996108899</v>
       </c>
       <c r="C16">
         <v>0.87746271403461995</v>
       </c>
       <c r="D16">
+        <v>0.87746271403461995</v>
+      </c>
+      <c r="E16">
         <v>1.7155711877451401</v>
-      </c>
-      <c r="E16">
-        <v>0.24879449996108899</v>
       </c>
       <c r="H16">
         <v>60</v>
@@ -23048,16 +23042,16 @@
         <v>65</v>
       </c>
       <c r="B17">
+        <v>0.28852395406988801</v>
+      </c>
+      <c r="C17">
         <v>0.67206293706674802</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>0.38554328942953098</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>4.6555048514850803</v>
-      </c>
-      <c r="E17">
-        <v>0.28852395406988801</v>
       </c>
       <c r="H17">
         <v>65</v>
@@ -23152,16 +23146,16 @@
         <v>70</v>
       </c>
       <c r="B18">
+        <v>0.33387481135659403</v>
+      </c>
+      <c r="C18">
         <v>2.22080465534951</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>2.8592022614041501</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>4.6555048514850803</v>
-      </c>
-      <c r="E18">
-        <v>0.33387481135659403</v>
       </c>
       <c r="H18">
         <v>70</v>
@@ -23256,16 +23250,16 @@
         <v>75</v>
       </c>
       <c r="B19">
+        <v>0.38554328942953098</v>
+      </c>
+      <c r="C19">
         <v>2.4174822379066199</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>0.87746271403461995</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>2.0388873079462901</v>
-      </c>
-      <c r="E19">
-        <v>0.38554328942953098</v>
       </c>
       <c r="H19">
         <v>75</v>
@@ -23360,16 +23354,16 @@
         <v>80</v>
       </c>
       <c r="B20">
+        <v>0.214058315601307</v>
+      </c>
+      <c r="C20">
         <v>1.87077681793044</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>0.38554328942953098</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>2.6299270915773598</v>
-      </c>
-      <c r="E20">
-        <v>0.214058315601307</v>
       </c>
       <c r="H20">
         <v>80</v>
@@ -23464,16 +23458,16 @@
         <v>85</v>
       </c>
       <c r="B21">
+        <v>0.28852395406988801</v>
+      </c>
+      <c r="C21">
         <v>1.87077681793044</v>
-      </c>
-      <c r="C21">
-        <v>2.6299270915773598</v>
       </c>
       <c r="D21">
         <v>2.6299270915773598</v>
       </c>
       <c r="E21">
-        <v>0.28852395406988801</v>
+        <v>2.6299270915773598</v>
       </c>
       <c r="H21">
         <v>85</v>
@@ -23568,16 +23562,16 @@
         <v>90</v>
       </c>
       <c r="B22">
+        <v>0.33387481135659403</v>
+      </c>
+      <c r="C22">
         <v>2.0388873079462901</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>0.76860885253802902</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>3.1064292267626299</v>
-      </c>
-      <c r="E22">
-        <v>0.33387481135659403</v>
       </c>
       <c r="H22">
         <v>90</v>
@@ -23672,16 +23666,16 @@
         <v>95</v>
       </c>
       <c r="B23">
+        <v>0.214058315601307</v>
+      </c>
+      <c r="C23">
         <v>1.1048704445411901</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>0.33387481135659403</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>3.65953171702269</v>
-      </c>
-      <c r="E23">
-        <v>0.214058315601307</v>
       </c>
       <c r="H23">
         <v>95</v>
@@ -23776,16 +23770,16 @@
         <v>100</v>
       </c>
       <c r="B24">
+        <v>0.24879449996108899</v>
+      </c>
+      <c r="C24">
         <v>1.2074340059003399</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>2.4174822379066199</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>1.2074340059003399</v>
-      </c>
-      <c r="E24">
-        <v>0.24879449996108899</v>
       </c>
       <c r="H24">
         <v>100</v>
@@ -23880,16 +23874,16 @@
         <v>105</v>
       </c>
       <c r="B25">
+        <v>0.28852395406988801</v>
+      </c>
+      <c r="C25">
         <v>0.87746271403461995</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>0.38554328942953098</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>3.9679652700759802</v>
-      </c>
-      <c r="E25">
-        <v>0.28852395406988801</v>
       </c>
       <c r="H25">
         <v>105</v>
@@ -23984,16 +23978,16 @@
         <v>110</v>
       </c>
       <c r="B26">
+        <v>0.24879449996108899</v>
+      </c>
+      <c r="C26">
         <v>1.1048704445411901</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>0.38554328942953098</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>3.1064292267626299</v>
-      </c>
-      <c r="E26">
-        <v>0.24879449996108899</v>
       </c>
       <c r="H26">
         <v>110</v>
@@ -24088,16 +24082,16 @@
         <v>115</v>
       </c>
       <c r="B27">
+        <v>0.33387481135659403</v>
+      </c>
+      <c r="C27">
         <v>2.4174822379066199</v>
       </c>
-      <c r="C27">
+      <c r="D27">
         <v>2.0388873079462901</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>1.7155711877451401</v>
-      </c>
-      <c r="E27">
-        <v>0.33387481135659403</v>
       </c>
       <c r="H27">
         <v>115</v>
@@ -24192,16 +24186,16 @@
         <v>120</v>
       </c>
       <c r="B28">
+        <v>0.24879449996108899</v>
+      </c>
+      <c r="C28">
         <v>2.0388873079462901</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>0.38554328942953098</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>2.4174822379066199</v>
-      </c>
-      <c r="E28">
-        <v>0.24879449996108899</v>
       </c>
       <c r="H28">
         <v>120</v>
@@ -24296,16 +24290,16 @@
         <v>125</v>
       </c>
       <c r="B29">
+        <v>0.28852395406988801</v>
+      </c>
+      <c r="C29">
         <v>1.87077681793044</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <v>2.22080465534951</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>2.4174822379066199</v>
-      </c>
-      <c r="E29">
-        <v>0.28852395406988801</v>
       </c>
       <c r="H29">
         <v>125</v>
@@ -24400,16 +24394,16 @@
         <v>130</v>
       </c>
       <c r="B30">
+        <v>0.38554328942953098</v>
+      </c>
+      <c r="C30">
         <v>1.87077681793044</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <v>0.87746271403461995</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>2.8592022614041501</v>
-      </c>
-      <c r="E30">
-        <v>0.38554328942953098</v>
       </c>
       <c r="H30">
         <v>130</v>
@@ -24504,16 +24498,16 @@
         <v>135</v>
       </c>
       <c r="B31">
+        <v>0.24879449996108899</v>
+      </c>
+      <c r="C31">
         <v>2.22080465534951</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <v>0.38554328942953098</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>3.1064292267626299</v>
-      </c>
-      <c r="E31">
-        <v>0.24879449996108899</v>
       </c>
       <c r="H31">
         <v>135</v>
@@ -24608,16 +24602,16 @@
         <v>140</v>
       </c>
       <c r="B32">
+        <v>0.33387481135659403</v>
+      </c>
+      <c r="C32">
         <v>1.0107600000000001</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <v>1.87077681793044</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>1.5724175935226301</v>
-      </c>
-      <c r="E32">
-        <v>0.33387481135659403</v>
       </c>
       <c r="H32">
         <v>140</v>
@@ -24712,16 +24706,16 @@
         <v>145</v>
       </c>
       <c r="B33">
-        <v>0.87746271403461995</v>
+        <v>0.38554328942953098</v>
       </c>
       <c r="C33">
         <v>0.87746271403461995</v>
       </c>
       <c r="D33">
+        <v>0.87746271403461995</v>
+      </c>
+      <c r="E33">
         <v>3.9679652700759802</v>
-      </c>
-      <c r="E33">
-        <v>0.38554328942953098</v>
       </c>
       <c r="H33">
         <v>145</v>
@@ -24816,16 +24810,16 @@
         <v>150</v>
       </c>
       <c r="B34">
+        <v>0.24879449996108899</v>
+      </c>
+      <c r="C34">
         <v>1.0107600000000001</v>
       </c>
-      <c r="C34">
+      <c r="D34">
         <v>0.38554328942953098</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>1.7155711877451401</v>
-      </c>
-      <c r="E34">
-        <v>0.24879449996108899</v>
       </c>
       <c r="H34">
         <v>150</v>
@@ -24920,16 +24914,16 @@
         <v>155</v>
       </c>
       <c r="B35">
-        <v>1.5724175935226301</v>
+        <v>0.33387481135659403</v>
       </c>
       <c r="C35">
         <v>1.5724175935226301</v>
       </c>
       <c r="D35">
+        <v>1.5724175935226301</v>
+      </c>
+      <c r="E35">
         <v>1.87077681793044</v>
-      </c>
-      <c r="E35">
-        <v>0.33387481135659403</v>
       </c>
       <c r="X35">
         <v>155</v>

</xml_diff>

<commit_message>
cap1. Estructura del documento + cambio figura 3.3
</commit_message>
<xml_diff>
--- a/datosDist.xlsx
+++ b/datosDist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MRS\Documents\Belen\ucm\5\TFG infor\git\TFG-1920-DiscapacidadVisual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58049402-019A-4BC9-A601-60A4FAF3B6E5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FC0A30-EA61-49F5-B0FD-6ACB468F1ABB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{BACB8FA7-8DF2-4461-B1D7-FE215F08741E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>beacon: CPne a 2m</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>beacon: Cpne a 64cm</t>
+  </si>
+  <si>
+    <t>beacon: eAaw a 1,5m</t>
   </si>
 </sst>
 </file>
@@ -4000,11 +4003,473 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="3"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
               <c:f>Hoja2!$I$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>beacon: eAaw a 7mm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja2!$H$5:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$I$5:$I$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>2.3869946426608699E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.1791219001070099E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.1791219001070099E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3869946426608699E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.1791219001070099E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3869946426608699E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.1791219001070099E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3869946426608699E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.62477979315498E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.1791219001070099E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.8775994811535699E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.3869946426608699E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.8614567472228602E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.8775994811535699E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.62477979315498E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.1791219001070099E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.8775994811535699E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.62477979315498E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.8775994811535699E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.8775994811535699E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.8775994811535699E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.8614567472228602E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.8775994811535699E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7.1791219001070099E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-DED3-4308-B51B-4340F7A958F1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>beacon: eAaw a 5cm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja2!$H$5:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$J$5:$J$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1.9729959084462598E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.08906436681886E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.62477979315498E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.62477979315498E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.08906436681886E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.62477979315498E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.9729959084462598E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.08906436681886E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.62477979315498E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.9729959084462598E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.62477979315498E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.08906436681886E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.8614567472228602E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.62477979315498E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.08906436681886E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.62477979315498E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.08906436681886E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DED3-4308-B51B-4340F7A958F1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$K$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4126,7 +4591,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja2!$I$5:$I$34</c:f>
+              <c:f>Hoja2!$K$5:$K$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -4232,14 +4697,14 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja2!$J$4</c:f>
+              <c:f>Hoja2!$L$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>beacon: eAaw a 0,5m</c:v>
+                  <c:v>beacon: eAaw a 1,5m</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4357,7 +4822,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja2!$J$5:$J$34</c:f>
+              <c:f>Hoja2!$L$5:$L$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -4458,468 +4923,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-DED3-4308-B51B-4340F7A958F1}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hoja2!$K$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>beacon: eAaw a 5cm</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Hoja2!$H$5:$H$34</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>115</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>125</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>135</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>150</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja2!$K$5:$K$34</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
-                <c:pt idx="0">
-                  <c:v>1.9729959084462598E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.3328853409862E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.3328853409862E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.08906436681886E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.3328853409862E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.62477979315498E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.3328853409862E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.62477979315498E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.08906436681886E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.3328853409862E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.62477979315498E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.3328853409862E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.3328853409862E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.9729959084462598E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.08906436681886E-2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.62477979315498E-2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.3328853409862E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.3328853409862E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.9729959084462598E-2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.3328853409862E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.3328853409862E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.62477979315498E-2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.08906436681886E-2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.3328853409862E-2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>8.8614567472228602E-3</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1.3328853409862E-2</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1.62477979315498E-2</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1.08906436681886E-2</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1.62477979315498E-2</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1.08906436681886E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-DED3-4308-B51B-4340F7A958F1}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hoja2!$L$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>beacon: eAaw a 7mm</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Hoja2!$H$5:$H$34</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>105</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>115</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>125</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>135</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>150</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja2!$L$5:$L$34</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
-                <c:pt idx="0">
-                  <c:v>2.3869946426608699E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.1791219001070099E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.1791219001070099E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.3869946426608699E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.1791219001070099E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.3869946426608699E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.3328853409862E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.1791219001070099E-3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.3869946426608699E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.62477979315498E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7.1791219001070099E-3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.8775994811535699E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.3328853409862E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2.3869946426608699E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.3328853409862E-2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>8.8614567472228602E-3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2.8775994811535699E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.62477979315498E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>7.1791219001070099E-3</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2.8775994811535699E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.62477979315498E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2.8775994811535699E-2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2.8775994811535699E-2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.3328853409862E-2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2.8775994811535699E-2</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1.3328853409862E-2</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>8.8614567472228602E-3</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2.8775994811535699E-2</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1.3328853409862E-2</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>7.1791219001070099E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-DED3-4308-B51B-4340F7A958F1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7558,6 +7561,1320 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES" sz="1600"/>
+              <a:t>beacon eAaw</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$I$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>beacon: eAaw a 7mm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja2!$H$5:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$I$5:$I$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>2.3869946426608699E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.1791219001070099E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.1791219001070099E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3869946426608699E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.1791219001070099E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3869946426608699E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.1791219001070099E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3869946426608699E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.62477979315498E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.1791219001070099E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.8775994811535699E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.3869946426608699E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.8614567472228602E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.8775994811535699E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.62477979315498E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.1791219001070099E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.8775994811535699E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.62477979315498E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.8775994811535699E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.8775994811535699E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.8775994811535699E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.8614567472228602E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.8775994811535699E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7.1791219001070099E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9F2F-4409-9385-5622533F3056}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>beacon: eAaw a 5cm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja2!$H$5:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$J$5:$J$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1.9729959084462598E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.08906436681886E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.62477979315498E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.62477979315498E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.08906436681886E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.62477979315498E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.9729959084462598E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.08906436681886E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.62477979315498E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.9729959084462598E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.62477979315498E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.08906436681886E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.8614567472228602E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.3328853409862E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.62477979315498E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.08906436681886E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.62477979315498E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.08906436681886E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9F2F-4409-9385-5622533F3056}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$K$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>beacon: eAaw a 0,5m</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja2!$H$5:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$K$5:$K$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1.0107600000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.67206293706674802</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.51099624947926003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0388873079462901</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.44429992043324701</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.51099624947926003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.58657202887224602</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.87746271403461995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.76860885253802902</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.67206293706674802</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.67206293706674802</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0107600000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3190883356183201</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1048704445411901</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1048704445411901</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.87746271403461995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.87746271403461995</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.87746271403461995</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.76860885253802902</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.67206293706674802</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.76860885253802902</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.67206293706674802</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.87746271403461995</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.76860885253802902</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.87746271403461995</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.76860885253802902</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.76860885253802902</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.87746271403461995</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.0107600000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.87746271403461995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9F2F-4409-9385-5622533F3056}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$L$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>beacon: eAaw a 1,5m</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja2!$H$5:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$L$5:$L$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1.5724175935226301</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.87746271403461995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1048704445411901</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.87746271403461995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7155711877451401</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.44051024859512</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.76860885253802902</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1048704445411901</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5724175935226301</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.87077681793044</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.3190883356183201</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.67206293706674802</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.1048704445411901</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1048704445411901</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.76860885253802902</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.1048704445411901</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.1048704445411901</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.67206293706674802</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.1048704445411901</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.2074340059003399</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.76860885253802902</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.3190883356183201</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.76860885253802902</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.76860885253802902</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.2074340059003399</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.76860885253802902</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.2074340059003399</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.44051024859512</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.87746271403461995</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.87746271403461995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9F2F-4409-9385-5622533F3056}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="511540008"/>
+        <c:axId val="511541320"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="511540008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES" sz="1600"/>
+                  <a:t>Tiempo (segundos)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="511541320"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="511541320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES" sz="1600"/>
+                  <a:t>Distancia (metros)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="511540008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="1.118083801906827E-2"/>
+          <c:y val="0.78445842388997178"/>
+          <c:w val="0.97168471874398277"/>
+          <c:h val="0.12661152887031704"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -7613,7 +8930,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja2!$I$4</c:f>
+              <c:f>Hoja2!$K$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7735,7 +9052,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja2!$I$5:$I$34</c:f>
+              <c:f>Hoja2!$K$5:$K$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -12232,6 +13549,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -16165,6 +17522,522 @@
 </file>
 
 <file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style17.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -21386,6 +23259,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>111126</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="16" name="Gráfico 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E5C2A3B-F13B-4B52-8BA7-7FF7328BC19F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -21688,8 +23597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD343F2-CB91-4D67-8970-030A01858BA8}">
   <dimension ref="A4:AX75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U83" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="Y99" sqref="Y99"/>
+    <sheetView tabSelected="1" topLeftCell="H112" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J139" sqref="J139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21735,16 +23644,16 @@
         <v>9</v>
       </c>
       <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" t="s">
         <v>13</v>
       </c>
-      <c r="J4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" t="s">
-        <v>12</v>
-      </c>
       <c r="L4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="P4" t="s">
         <v>1</v>
@@ -21809,16 +23718,16 @@
         <v>5</v>
       </c>
       <c r="I5">
+        <v>2.3869946426608699E-2</v>
+      </c>
+      <c r="J5">
+        <v>1.9729959084462598E-2</v>
+      </c>
+      <c r="K5">
         <v>1.0107600000000001</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>1.5724175935226301</v>
-      </c>
-      <c r="K5">
-        <v>1.9729959084462598E-2</v>
-      </c>
-      <c r="L5">
-        <v>2.3869946426608699E-2</v>
       </c>
       <c r="O5">
         <v>5</v>
@@ -21913,16 +23822,16 @@
         <v>10</v>
       </c>
       <c r="I6">
+        <v>7.1791219001070099E-3</v>
+      </c>
+      <c r="J6">
+        <v>1.3328853409862E-2</v>
+      </c>
+      <c r="K6">
         <v>0.67206293706674802</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>0.87746271403461995</v>
-      </c>
-      <c r="K6">
-        <v>1.3328853409862E-2</v>
-      </c>
-      <c r="L6">
-        <v>7.1791219001070099E-3</v>
       </c>
       <c r="O6">
         <v>10</v>
@@ -22017,16 +23926,16 @@
         <v>15</v>
       </c>
       <c r="I7">
+        <v>7.1791219001070099E-3</v>
+      </c>
+      <c r="J7">
+        <v>1.3328853409862E-2</v>
+      </c>
+      <c r="K7">
         <v>0.51099624947926003</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>1.1048704445411901</v>
-      </c>
-      <c r="K7">
-        <v>1.3328853409862E-2</v>
-      </c>
-      <c r="L7">
-        <v>7.1791219001070099E-3</v>
       </c>
       <c r="O7">
         <v>15</v>
@@ -22121,16 +24030,16 @@
         <v>20</v>
       </c>
       <c r="I8">
+        <v>2.3869946426608699E-2</v>
+      </c>
+      <c r="J8">
+        <v>1.08906436681886E-2</v>
+      </c>
+      <c r="K8">
         <v>2.0388873079462901</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>0.87746271403461995</v>
-      </c>
-      <c r="K8">
-        <v>1.08906436681886E-2</v>
-      </c>
-      <c r="L8">
-        <v>2.3869946426608699E-2</v>
       </c>
       <c r="O8">
         <v>20</v>
@@ -22225,16 +24134,16 @@
         <v>25</v>
       </c>
       <c r="I9">
+        <v>7.1791219001070099E-3</v>
+      </c>
+      <c r="J9">
+        <v>1.3328853409862E-2</v>
+      </c>
+      <c r="K9">
         <v>0.44429992043324701</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>1.7155711877451401</v>
-      </c>
-      <c r="K9">
-        <v>1.3328853409862E-2</v>
-      </c>
-      <c r="L9">
-        <v>7.1791219001070099E-3</v>
       </c>
       <c r="O9">
         <v>25</v>
@@ -22329,16 +24238,16 @@
         <v>30</v>
       </c>
       <c r="I10">
+        <v>2.3869946426608699E-2</v>
+      </c>
+      <c r="J10">
+        <v>1.62477979315498E-2</v>
+      </c>
+      <c r="K10">
         <v>0.51099624947926003</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>1.44051024859512</v>
-      </c>
-      <c r="K10">
-        <v>1.62477979315498E-2</v>
-      </c>
-      <c r="L10">
-        <v>2.3869946426608699E-2</v>
       </c>
       <c r="O10">
         <v>30</v>
@@ -22433,16 +24342,16 @@
         <v>35</v>
       </c>
       <c r="I11">
+        <v>1.3328853409862E-2</v>
+      </c>
+      <c r="J11">
+        <v>1.3328853409862E-2</v>
+      </c>
+      <c r="K11">
         <v>0.58657202887224602</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>0.76860885253802902</v>
-      </c>
-      <c r="K11">
-        <v>1.3328853409862E-2</v>
-      </c>
-      <c r="L11">
-        <v>1.3328853409862E-2</v>
       </c>
       <c r="O11">
         <v>35</v>
@@ -22537,16 +24446,16 @@
         <v>40</v>
       </c>
       <c r="I12">
+        <v>7.1791219001070099E-3</v>
+      </c>
+      <c r="J12">
+        <v>1.62477979315498E-2</v>
+      </c>
+      <c r="K12">
         <v>0.87746271403461995</v>
       </c>
-      <c r="J12">
+      <c r="L12">
         <v>1.1048704445411901</v>
-      </c>
-      <c r="K12">
-        <v>1.62477979315498E-2</v>
-      </c>
-      <c r="L12">
-        <v>7.1791219001070099E-3</v>
       </c>
       <c r="O12">
         <v>40</v>
@@ -22641,16 +24550,16 @@
         <v>45</v>
       </c>
       <c r="I13">
+        <v>2.3869946426608699E-2</v>
+      </c>
+      <c r="J13">
+        <v>1.08906436681886E-2</v>
+      </c>
+      <c r="K13">
         <v>0.76860885253802902</v>
       </c>
-      <c r="J13">
+      <c r="L13">
         <v>1.5724175935226301</v>
-      </c>
-      <c r="K13">
-        <v>1.08906436681886E-2</v>
-      </c>
-      <c r="L13">
-        <v>2.3869946426608699E-2</v>
       </c>
       <c r="O13">
         <v>45</v>
@@ -22745,16 +24654,16 @@
         <v>50</v>
       </c>
       <c r="I14">
+        <v>1.62477979315498E-2</v>
+      </c>
+      <c r="J14">
+        <v>1.3328853409862E-2</v>
+      </c>
+      <c r="K14">
         <v>0.67206293706674802</v>
       </c>
-      <c r="J14">
+      <c r="L14">
         <v>1.87077681793044</v>
-      </c>
-      <c r="K14">
-        <v>1.3328853409862E-2</v>
-      </c>
-      <c r="L14">
-        <v>1.62477979315498E-2</v>
       </c>
       <c r="O14">
         <v>50</v>
@@ -22849,16 +24758,16 @@
         <v>55</v>
       </c>
       <c r="I15">
+        <v>7.1791219001070099E-3</v>
+      </c>
+      <c r="J15">
+        <v>1.62477979315498E-2</v>
+      </c>
+      <c r="K15">
         <v>0.67206293706674802</v>
       </c>
-      <c r="J15">
+      <c r="L15">
         <v>1.3190883356183201</v>
-      </c>
-      <c r="K15">
-        <v>1.62477979315498E-2</v>
-      </c>
-      <c r="L15">
-        <v>7.1791219001070099E-3</v>
       </c>
       <c r="O15">
         <v>55</v>
@@ -22953,16 +24862,16 @@
         <v>60</v>
       </c>
       <c r="I16">
+        <v>2.8775994811535699E-2</v>
+      </c>
+      <c r="J16">
+        <v>1.3328853409862E-2</v>
+      </c>
+      <c r="K16">
         <v>1.0107600000000001</v>
       </c>
-      <c r="J16">
+      <c r="L16">
         <v>0.67206293706674802</v>
-      </c>
-      <c r="K16">
-        <v>1.3328853409862E-2</v>
-      </c>
-      <c r="L16">
-        <v>2.8775994811535699E-2</v>
       </c>
       <c r="O16">
         <v>60</v>
@@ -23057,16 +24966,16 @@
         <v>65</v>
       </c>
       <c r="I17">
+        <v>1.3328853409862E-2</v>
+      </c>
+      <c r="J17">
+        <v>1.3328853409862E-2</v>
+      </c>
+      <c r="K17">
         <v>1.3190883356183201</v>
       </c>
-      <c r="J17">
+      <c r="L17">
         <v>1.1048704445411901</v>
-      </c>
-      <c r="K17">
-        <v>1.3328853409862E-2</v>
-      </c>
-      <c r="L17">
-        <v>1.3328853409862E-2</v>
       </c>
       <c r="O17">
         <v>65</v>
@@ -23161,16 +25070,16 @@
         <v>70</v>
       </c>
       <c r="I18">
+        <v>2.3869946426608699E-2</v>
+      </c>
+      <c r="J18">
+        <v>1.9729959084462598E-2</v>
+      </c>
+      <c r="K18">
         <v>1.1048704445411901</v>
       </c>
-      <c r="J18">
+      <c r="L18">
         <v>1.1048704445411901</v>
-      </c>
-      <c r="K18">
-        <v>1.9729959084462598E-2</v>
-      </c>
-      <c r="L18">
-        <v>2.3869946426608699E-2</v>
       </c>
       <c r="O18">
         <v>70</v>
@@ -23265,16 +25174,16 @@
         <v>75</v>
       </c>
       <c r="I19">
+        <v>1.3328853409862E-2</v>
+      </c>
+      <c r="J19">
+        <v>1.08906436681886E-2</v>
+      </c>
+      <c r="K19">
         <v>1.1048704445411901</v>
       </c>
-      <c r="J19">
+      <c r="L19">
         <v>0.76860885253802902</v>
-      </c>
-      <c r="K19">
-        <v>1.08906436681886E-2</v>
-      </c>
-      <c r="L19">
-        <v>1.3328853409862E-2</v>
       </c>
       <c r="O19">
         <v>75</v>
@@ -23369,16 +25278,16 @@
         <v>80</v>
       </c>
       <c r="I20">
+        <v>8.8614567472228602E-3</v>
+      </c>
+      <c r="J20">
+        <v>1.62477979315498E-2</v>
+      </c>
+      <c r="K20">
         <v>0.87746271403461995</v>
       </c>
-      <c r="J20">
+      <c r="L20">
         <v>1.1048704445411901</v>
-      </c>
-      <c r="K20">
-        <v>1.62477979315498E-2</v>
-      </c>
-      <c r="L20">
-        <v>8.8614567472228602E-3</v>
       </c>
       <c r="O20">
         <v>80</v>
@@ -23473,16 +25382,16 @@
         <v>85</v>
       </c>
       <c r="I21">
+        <v>2.8775994811535699E-2</v>
+      </c>
+      <c r="J21">
+        <v>1.3328853409862E-2</v>
+      </c>
+      <c r="K21">
         <v>0.87746271403461995</v>
       </c>
-      <c r="J21">
+      <c r="L21">
         <v>1.1048704445411901</v>
-      </c>
-      <c r="K21">
-        <v>1.3328853409862E-2</v>
-      </c>
-      <c r="L21">
-        <v>2.8775994811535699E-2</v>
       </c>
       <c r="O21">
         <v>85</v>
@@ -23577,16 +25486,16 @@
         <v>90</v>
       </c>
       <c r="I22">
+        <v>1.62477979315498E-2</v>
+      </c>
+      <c r="J22">
+        <v>1.3328853409862E-2</v>
+      </c>
+      <c r="K22">
         <v>0.87746271403461995</v>
       </c>
-      <c r="J22">
+      <c r="L22">
         <v>0.67206293706674802</v>
-      </c>
-      <c r="K22">
-        <v>1.3328853409862E-2</v>
-      </c>
-      <c r="L22">
-        <v>1.62477979315498E-2</v>
       </c>
       <c r="O22">
         <v>90</v>
@@ -23681,16 +25590,16 @@
         <v>95</v>
       </c>
       <c r="I23">
+        <v>7.1791219001070099E-3</v>
+      </c>
+      <c r="J23">
+        <v>1.9729959084462598E-2</v>
+      </c>
+      <c r="K23">
         <v>0.76860885253802902</v>
       </c>
-      <c r="J23">
+      <c r="L23">
         <v>1.1048704445411901</v>
-      </c>
-      <c r="K23">
-        <v>1.9729959084462598E-2</v>
-      </c>
-      <c r="L23">
-        <v>7.1791219001070099E-3</v>
       </c>
       <c r="O23">
         <v>95</v>
@@ -23785,16 +25694,16 @@
         <v>100</v>
       </c>
       <c r="I24">
+        <v>2.8775994811535699E-2</v>
+      </c>
+      <c r="J24">
+        <v>1.3328853409862E-2</v>
+      </c>
+      <c r="K24">
         <v>0.67206293706674802</v>
       </c>
-      <c r="J24">
+      <c r="L24">
         <v>1.2074340059003399</v>
-      </c>
-      <c r="K24">
-        <v>1.3328853409862E-2</v>
-      </c>
-      <c r="L24">
-        <v>2.8775994811535699E-2</v>
       </c>
       <c r="O24">
         <v>100</v>
@@ -23889,16 +25798,16 @@
         <v>105</v>
       </c>
       <c r="I25">
+        <v>1.62477979315498E-2</v>
+      </c>
+      <c r="J25">
+        <v>1.3328853409862E-2</v>
+      </c>
+      <c r="K25">
         <v>0.76860885253802902</v>
       </c>
-      <c r="J25">
+      <c r="L25">
         <v>0.76860885253802902</v>
-      </c>
-      <c r="K25">
-        <v>1.3328853409862E-2</v>
-      </c>
-      <c r="L25">
-        <v>1.62477979315498E-2</v>
       </c>
       <c r="O25">
         <v>105</v>
@@ -23993,16 +25902,16 @@
         <v>110</v>
       </c>
       <c r="I26">
+        <v>2.8775994811535699E-2</v>
+      </c>
+      <c r="J26">
+        <v>1.62477979315498E-2</v>
+      </c>
+      <c r="K26">
         <v>0.67206293706674802</v>
       </c>
-      <c r="J26">
+      <c r="L26">
         <v>1.3190883356183201</v>
-      </c>
-      <c r="K26">
-        <v>1.62477979315498E-2</v>
-      </c>
-      <c r="L26">
-        <v>2.8775994811535699E-2</v>
       </c>
       <c r="O26">
         <v>110</v>
@@ -24097,16 +26006,16 @@
         <v>115</v>
       </c>
       <c r="I27">
+        <v>2.8775994811535699E-2</v>
+      </c>
+      <c r="J27">
+        <v>1.08906436681886E-2</v>
+      </c>
+      <c r="K27">
         <v>0.87746271403461995</v>
       </c>
-      <c r="J27">
+      <c r="L27">
         <v>0.76860885253802902</v>
-      </c>
-      <c r="K27">
-        <v>1.08906436681886E-2</v>
-      </c>
-      <c r="L27">
-        <v>2.8775994811535699E-2</v>
       </c>
       <c r="O27">
         <v>115</v>
@@ -24201,16 +26110,16 @@
         <v>120</v>
       </c>
       <c r="I28">
+        <v>1.3328853409862E-2</v>
+      </c>
+      <c r="J28">
+        <v>1.3328853409862E-2</v>
+      </c>
+      <c r="K28">
         <v>0.76860885253802902</v>
       </c>
-      <c r="J28">
+      <c r="L28">
         <v>0.76860885253802902</v>
-      </c>
-      <c r="K28">
-        <v>1.3328853409862E-2</v>
-      </c>
-      <c r="L28">
-        <v>1.3328853409862E-2</v>
       </c>
       <c r="O28">
         <v>120</v>
@@ -24305,16 +26214,16 @@
         <v>125</v>
       </c>
       <c r="I29">
+        <v>2.8775994811535699E-2</v>
+      </c>
+      <c r="J29">
+        <v>8.8614567472228602E-3</v>
+      </c>
+      <c r="K29">
         <v>0.87746271403461995</v>
       </c>
-      <c r="J29">
+      <c r="L29">
         <v>1.2074340059003399</v>
-      </c>
-      <c r="K29">
-        <v>8.8614567472228602E-3</v>
-      </c>
-      <c r="L29">
-        <v>2.8775994811535699E-2</v>
       </c>
       <c r="O29">
         <v>125</v>
@@ -24409,16 +26318,16 @@
         <v>130</v>
       </c>
       <c r="I30">
+        <v>1.3328853409862E-2</v>
+      </c>
+      <c r="J30">
+        <v>1.3328853409862E-2</v>
+      </c>
+      <c r="K30">
         <v>0.76860885253802902</v>
       </c>
-      <c r="J30">
+      <c r="L30">
         <v>0.76860885253802902</v>
-      </c>
-      <c r="K30">
-        <v>1.3328853409862E-2</v>
-      </c>
-      <c r="L30">
-        <v>1.3328853409862E-2</v>
       </c>
       <c r="O30">
         <v>130</v>
@@ -24513,16 +26422,16 @@
         <v>135</v>
       </c>
       <c r="I31">
+        <v>8.8614567472228602E-3</v>
+      </c>
+      <c r="J31">
+        <v>1.62477979315498E-2</v>
+      </c>
+      <c r="K31">
         <v>0.76860885253802902</v>
       </c>
-      <c r="J31">
+      <c r="L31">
         <v>1.2074340059003399</v>
-      </c>
-      <c r="K31">
-        <v>1.62477979315498E-2</v>
-      </c>
-      <c r="L31">
-        <v>8.8614567472228602E-3</v>
       </c>
       <c r="O31">
         <v>135</v>
@@ -24617,16 +26526,16 @@
         <v>140</v>
       </c>
       <c r="I32">
+        <v>2.8775994811535699E-2</v>
+      </c>
+      <c r="J32">
+        <v>1.08906436681886E-2</v>
+      </c>
+      <c r="K32">
         <v>0.87746271403461995</v>
       </c>
-      <c r="J32">
+      <c r="L32">
         <v>1.44051024859512</v>
-      </c>
-      <c r="K32">
-        <v>1.08906436681886E-2</v>
-      </c>
-      <c r="L32">
-        <v>2.8775994811535699E-2</v>
       </c>
       <c r="O32">
         <v>140</v>
@@ -24721,16 +26630,16 @@
         <v>145</v>
       </c>
       <c r="I33">
+        <v>1.3328853409862E-2</v>
+      </c>
+      <c r="J33">
+        <v>1.62477979315498E-2</v>
+      </c>
+      <c r="K33">
         <v>1.0107600000000001</v>
       </c>
-      <c r="J33">
+      <c r="L33">
         <v>0.87746271403461995</v>
-      </c>
-      <c r="K33">
-        <v>1.62477979315498E-2</v>
-      </c>
-      <c r="L33">
-        <v>1.3328853409862E-2</v>
       </c>
       <c r="O33">
         <v>145</v>
@@ -24825,16 +26734,16 @@
         <v>150</v>
       </c>
       <c r="I34">
+        <v>7.1791219001070099E-3</v>
+      </c>
+      <c r="J34">
+        <v>1.08906436681886E-2</v>
+      </c>
+      <c r="K34">
         <v>0.87746271403461995</v>
       </c>
-      <c r="J34">
+      <c r="L34">
         <v>0.87746271403461995</v>
-      </c>
-      <c r="K34">
-        <v>1.08906436681886E-2</v>
-      </c>
-      <c r="L34">
-        <v>7.1791219001070099E-3</v>
       </c>
       <c r="O34">
         <v>150</v>

</xml_diff>